<commit_message>
insert new figures n timeline into pp
</commit_message>
<xml_diff>
--- a/Deliverables/sSQA.xlsx
+++ b/Deliverables/sSQA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmusherskind/ITU/Architecture/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgrum\Documents\Programming\Architecture\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCA0CF0-BAF8-3843-9BA5-19ED2E97243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D063210-BC3A-43AF-B944-50186767E1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="3780" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16200" yWindow="1335" windowWidth="16755" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -298,7 +299,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -378,7 +379,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Performance</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -394,27 +395,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>[1]Sheet1!$D$8:$D$12</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Event Broker</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Odds Updater</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Actor model</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Load Balancer</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Combo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -423,19 +425,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,7 +457,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Modifiability</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -471,27 +473,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>[1]Sheet1!$D$8:$D$12</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Event Broker</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Odds Updater</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Actor model</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Load Balancer</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Combo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -500,19 +503,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,7 +535,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Safety</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -548,27 +551,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>[1]Sheet1!$D$8:$D$12</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Event Broker</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Odds Updater</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Actor model</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Load Balancer</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Combo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -577,19 +581,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,7 +801,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -854,7 +858,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Commulative</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -870,27 +874,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>[1]Sheet1!$D$8:$D$12</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Event Broker</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Odds Updater</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Actor model</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Load Balancer</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Combo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -899,19 +904,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2283,6 +2288,19 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -2295,20 +2313,8 @@
           <cell r="E7" t="str">
             <v>Performance</v>
           </cell>
-          <cell r="F7" t="str">
-            <v>Modifiability</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>Safety</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>Commulative</v>
-          </cell>
         </row>
         <row r="8">
-          <cell r="D8" t="str">
-            <v>Event Broker</v>
-          </cell>
           <cell r="E8">
             <v>2</v>
           </cell>
@@ -2323,9 +2329,6 @@
           </cell>
         </row>
         <row r="9">
-          <cell r="D9" t="str">
-            <v>Odds Updater</v>
-          </cell>
           <cell r="E9">
             <v>4</v>
           </cell>
@@ -2340,9 +2343,6 @@
           </cell>
         </row>
         <row r="10">
-          <cell r="D10" t="str">
-            <v>Actor model</v>
-          </cell>
           <cell r="E10">
             <v>4</v>
           </cell>
@@ -2357,9 +2357,6 @@
           </cell>
         </row>
         <row r="11">
-          <cell r="D11" t="str">
-            <v>Load Balancer</v>
-          </cell>
           <cell r="E11">
             <v>4</v>
           </cell>
@@ -2374,9 +2371,6 @@
           </cell>
         </row>
         <row r="12">
-          <cell r="D12" t="str">
-            <v>Combo</v>
-          </cell>
           <cell r="E12">
             <v>4</v>
           </cell>
@@ -2661,32 +2655,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BB54"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="79" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="79" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="35" max="35" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" customWidth="1"/>
     <col min="36" max="36" width="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="39" max="40" width="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="2.5" customWidth="1"/>
+    <col min="41" max="41" width="2.42578125" customWidth="1"/>
     <col min="42" max="42" width="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="46" width="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="2.5" customWidth="1"/>
+    <col min="47" max="47" width="2.42578125" customWidth="1"/>
     <col min="48" max="48" width="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
@@ -2699,7 +2693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2719,7 +2713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2727,24 +2721,24 @@
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="4">
         <f>5-MAX(0,C3-D3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
       </c>
       <c r="G3" s="4">
         <f>_xlfn.CEILING.MATH((6-E3)*F3/5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2769,7 +2763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2791,7 +2785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2813,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2835,7 +2829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2845,7 +2839,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2865,7 +2859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -2887,7 +2881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -2909,7 +2903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2917,24 +2911,24 @@
         <v>4</v>
       </c>
       <c r="D13" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" s="4">
         <v>4</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2942,21 +2936,21 @@
         <v>4</v>
       </c>
       <c r="D14" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4">
         <v>4</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2964,24 +2958,24 @@
         <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4">
         <v>4</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
@@ -2991,7 +2985,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -3014,7 +3008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -3039,7 +3033,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3061,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3069,21 +3063,21 @@
         <v>4</v>
       </c>
       <c r="D21" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F21" s="4">
         <v>5</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3091,24 +3085,24 @@
         <v>4</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22" s="4">
         <v>5</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3130,7 +3124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>15</v>
       </c>
@@ -3140,7 +3134,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
@@ -3160,7 +3154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
@@ -3176,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>7</v>
       </c>
@@ -3192,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3208,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
@@ -3226,7 +3220,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
@@ -3242,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>16</v>
       </c>
@@ -3252,7 +3246,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="2:52" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:52" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
@@ -3272,7 +3266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:52" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
@@ -3288,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:52" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
@@ -3304,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:52" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:52" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
@@ -3323,7 +3317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:52" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
@@ -3341,7 +3335,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="39" spans="2:52" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:52" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>10</v>
       </c>
@@ -3357,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:52" x14ac:dyDescent="0.25">
       <c r="AJ48" t="s">
         <v>12</v>
       </c>
@@ -3376,7 +3370,7 @@
       <c r="AY48" s="6"/>
       <c r="AZ48" s="6"/>
     </row>
-    <row r="49" spans="35:54" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="35:54" x14ac:dyDescent="0.25">
       <c r="AI49" s="1" t="s">
         <v>0</v>
       </c>
@@ -3426,7 +3420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="35:54" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="35:54" x14ac:dyDescent="0.25">
       <c r="AI50" s="2" t="s">
         <v>6</v>
       </c>
@@ -3482,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="35:54" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="35:54" ht="30" x14ac:dyDescent="0.25">
       <c r="AI51" s="2" t="s">
         <v>7</v>
       </c>
@@ -3541,7 +3535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="35:54" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="35:54" ht="30" x14ac:dyDescent="0.25">
       <c r="AI52" s="2" t="s">
         <v>8</v>
       </c>
@@ -3600,7 +3594,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="35:54" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="35:54" ht="30" x14ac:dyDescent="0.25">
       <c r="AI53" s="2" t="s">
         <v>9</v>
       </c>
@@ -3656,7 +3650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="35:54" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="35:54" ht="45" x14ac:dyDescent="0.25">
       <c r="AI54" s="2" t="s">
         <v>10</v>
       </c>
@@ -3734,13 +3728,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD781A43-2393-7249-BAD4-C623455F7A3A}">
   <dimension ref="E6:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+    <sheetView zoomScale="67" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="5:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3760,7 +3754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>6</v>
       </c>
@@ -3778,7 +3772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>7</v>
       </c>
@@ -3796,7 +3790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>35</v>
       </c>
@@ -3814,7 +3808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>9</v>
       </c>
@@ -3832,7 +3826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>36</v>
       </c>

</xml_diff>